<commit_message>
created test data for Valid Login Test script
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B120 6AM Selenium\share\Day21_07_01_2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\b120afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03E8923-E0BE-484A-8E82-640271BD9620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A36E6-F509-4522-A75D-02D5267396CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>akshara</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -345,17 +354,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Drive Invalid Login Test Script
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\b120afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A36E6-F509-4522-A75D-02D5267396CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1E78C6-8B40-4619-AD5C-C78C8D04AF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>admin</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -60,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,12 +75,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,29 +379,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159111D0-DEA8-4777-BBC0-0249CF97A07F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>